<commit_message>
fix feuille pointage documents
</commit_message>
<xml_diff>
--- a/documents/Model Feuille de pointages 2018.xlsx
+++ b/documents/Model Feuille de pointages 2018.xlsx
@@ -306,7 +306,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -439,11 +439,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -480,9 +561,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -492,33 +570,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -529,6 +580,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,7 +650,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:colOff>552450</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -881,7 +974,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,8 +982,8 @@
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" customWidth="1"/>
     <col min="8" max="8" width="11.140625" customWidth="1"/>
@@ -904,20 +997,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="29"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
+      <c r="A1" s="35"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
@@ -968,22 +1061,22 @@
       <c r="N4" s="3"/>
     </row>
     <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="30"/>
-      <c r="L5" s="30"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="30"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+      <c r="M5" s="36"/>
+      <c r="N5" s="36"/>
     </row>
     <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="E6" s="1"/>
@@ -1012,11 +1105,11 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -1030,11 +1123,11 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
       <c r="D9" s="6"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -1076,14 +1169,14 @@
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="1"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="37" t="s">
+      <c r="I11" s="25"/>
+      <c r="J11" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="36" t="s">
+      <c r="K11" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="L11" s="38" t="s">
+      <c r="L11" s="28" t="s">
         <v>31</v>
       </c>
       <c r="M11" s="1"/>
@@ -1124,50 +1217,50 @@
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:14" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="H14" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="26" t="s">
+      <c r="I14" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="33" t="s">
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="31" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="33"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
+      <c r="A15" s="31"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
       <c r="I15" s="9" t="s">
         <v>20</v>
       </c>
@@ -1183,9 +1276,9 @@
       <c r="M15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="N15" s="33"/>
-    </row>
-    <row r="16" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N15" s="31"/>
+    </row>
+    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -1205,14 +1298,14 @@
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>
     </row>
-    <row r="17" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="19">
+    <row r="17" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="38">
         <v>2</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="15"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -1225,14 +1318,14 @@
       <c r="M17" s="15"/>
       <c r="N17" s="15"/>
     </row>
-    <row r="18" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16">
+    <row r="18" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="43">
         <v>3</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="17"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
@@ -1246,13 +1339,13 @@
       <c r="N18" s="17"/>
     </row>
     <row r="19" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
+      <c r="A19" s="38">
         <v>4</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="15"/>
+      <c r="C19" s="40"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -1266,13 +1359,13 @@
       <c r="N19" s="15"/>
     </row>
     <row r="20" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20">
+      <c r="A20" s="39">
         <v>5</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="18"/>
+      <c r="C20" s="41"/>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
@@ -1366,131 +1459,135 @@
       <c r="N24" s="14"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
     </row>
     <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
     </row>
     <row r="27" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
+      <c r="A27" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="32"/>
-      <c r="N27" s="32"/>
-      <c r="O27" s="32"/>
-      <c r="P27" s="32"/>
-      <c r="Q27" s="32"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="30"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
     </row>
     <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
       <c r="L28" s="8" t="s">
         <v>12</v>
       </c>
       <c r="M28" s="8"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
     </row>
     <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
       <c r="H29" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="25"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="22"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="22"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="31"/>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
+      <c r="A31" s="29"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A5:N5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
     <mergeCell ref="A31:K31"/>
     <mergeCell ref="A27:Q27"/>
     <mergeCell ref="A28:I28"/>
@@ -1505,10 +1602,6 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="F14:F15"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A5:N5"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Add type de contrat
</commit_message>
<xml_diff>
--- a/documents/Model Feuille de pointages 2018.xlsx
+++ b/documents/Model Feuille de pointages 2018.xlsx
@@ -24,7 +24,7 @@
     <sheet name="Feuil10" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$O$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$N$34</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Etat de Présence mensuel</t>
-  </si>
-  <si>
-    <t>(**)Portez la mention appropriée:période de congé de maladie,maternité,accident de travail,congé annuel,,,,,ect</t>
   </si>
   <si>
     <t>N°</t>
@@ -223,12 +220,15 @@
   <si>
     <t>https://anem.info/#/download</t>
   </si>
+  <si>
+    <t>(**)Portez la mention appropriée:période de congé de maladie,maternité,accident de travail,congé annuel...ect</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,6 +317,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -326,7 +335,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -410,51 +419,6 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -545,7 +509,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -591,31 +555,33 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -634,17 +600,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -666,7 +633,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -675,35 +642,119 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:colOff>704850</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="1027" name="Group 3"/>
+        <xdr:cNvGrpSpPr>
+          <a:grpSpLocks noChangeAspect="1"/>
+        </xdr:cNvGrpSpPr>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr bwMode="auto">
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10287000" cy="971550"/>
+          <a:ext cx="10839450" cy="971550"/>
+          <a:chOff x="0" y="0"/>
+          <a:chExt cx="1080" cy="102"/>
         </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="1026" name="AutoShape 2"/>
+          <xdr:cNvSpPr>
+            <a:spLocks noChangeAspect="1" noChangeArrowheads="1" noTextEdit="1"/>
+          </xdr:cNvSpPr>
+        </xdr:nvSpPr>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="1080" cy="102"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+            <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:miter lim="800000"/>
+                <a:headEnd/>
+                <a:tailEnd/>
+              </a14:hiddenLine>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:sp>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="5" name="Image 4"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="1081" cy="103"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+            <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:miter lim="800000"/>
+                <a:headEnd/>
+                <a:tailEnd/>
+              </a14:hiddenLine>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -996,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,21 +1058,20 @@
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="36"/>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
@@ -1035,15 +1085,14 @@
       <c r="K1" s="36"/>
       <c r="L1" s="36"/>
       <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-    </row>
-    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="5"/>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -1051,15 +1100,14 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="5"/>
       <c r="C3" s="3"/>
       <c r="D3" s="4"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="4"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -1067,15 +1115,14 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-    </row>
-    <row r="4" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="5"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -1083,12 +1130,9 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-    </row>
-    <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="37" t="s">
-        <v>2</v>
-      </c>
+    </row>
+    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="37"/>
       <c r="B5" s="37"/>
       <c r="C5" s="37"/>
       <c r="D5" s="37"/>
@@ -1101,222 +1145,209 @@
       <c r="K5" s="37"/>
       <c r="L5" s="37"/>
       <c r="M5" s="37"/>
-      <c r="N5" s="37"/>
-    </row>
-    <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
+    </row>
+    <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="I6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
+      <c r="L6" s="1"/>
       <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
+      <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A9" s="38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
       <c r="D9" s="6"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="1"/>
+      <c r="F9" s="45" t="s">
+        <v>2</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
+      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="K11" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="L11" s="28" t="s">
-        <v>31</v>
-      </c>
+      <c r="G11" s="1"/>
+      <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="46" t="s">
+        <v>13</v>
+      </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
+      <c r="J12" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="43" t="s">
+        <v>30</v>
+      </c>
       <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="44"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:13" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="41" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="42" t="s">
+      <c r="G14" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="I14" s="42" t="s">
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="41" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="41"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L15" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="41" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="41"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="L15" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="M15" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="N15" s="41"/>
-    </row>
-    <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M15" s="41"/>
+    </row>
+    <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>1</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
+      <c r="D16" s="12">
+        <v>43101</v>
+      </c>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
@@ -1326,16 +1357,15 @@
       <c r="K16" s="11"/>
       <c r="L16" s="11"/>
       <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-    </row>
-    <row r="17" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29">
+    </row>
+    <row r="17" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="25">
         <v>2</v>
       </c>
-      <c r="B17" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="31"/>
+      <c r="B17" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="27"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -1346,16 +1376,15 @@
       <c r="K17" s="15"/>
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
-      <c r="N17" s="15"/>
-    </row>
-    <row r="18" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34">
+    </row>
+    <row r="18" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="30">
         <v>3</v>
       </c>
-      <c r="B18" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="35"/>
+      <c r="B18" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="31"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
@@ -1366,16 +1395,15 @@
       <c r="K18" s="17"/>
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-    </row>
-    <row r="19" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="29">
+    </row>
+    <row r="19" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="25">
         <v>4</v>
       </c>
-      <c r="B19" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="31"/>
+      <c r="B19" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="27"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -1386,16 +1414,15 @@
       <c r="K19" s="15"/>
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-    </row>
-    <row r="20" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30">
+    </row>
+    <row r="20" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="26">
         <v>5</v>
       </c>
-      <c r="B20" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="32"/>
+      <c r="B20" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="28"/>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18"/>
@@ -1406,14 +1433,13 @@
       <c r="K20" s="18"/>
       <c r="L20" s="18"/>
       <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-    </row>
-    <row r="21" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16">
         <v>6</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -1426,14 +1452,13 @@
       <c r="K21" s="17"/>
       <c r="L21" s="17"/>
       <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-    </row>
-    <row r="22" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>7</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
@@ -1446,14 +1471,13 @@
       <c r="K22" s="15"/>
       <c r="L22" s="15"/>
       <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-    </row>
-    <row r="23" spans="1:17" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>8</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -1466,14 +1490,13 @@
       <c r="K23" s="15"/>
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-    </row>
-    <row r="24" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13">
         <v>9</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
@@ -1486,18 +1509,17 @@
       <c r="K24" s="14"/>
       <c r="L24" s="14"/>
       <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
-    </row>
-    <row r="25" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
+      <c r="G25" s="22"/>
       <c r="H25" s="22"/>
       <c r="I25" s="22"/>
       <c r="J25" s="22"/>
@@ -1507,11 +1529,10 @@
       <c r="N25" s="22"/>
       <c r="O25" s="22"/>
       <c r="P25" s="22"/>
-      <c r="Q25" s="22"/>
-    </row>
-    <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B26" s="40"/>
       <c r="C26" s="40"/>
@@ -1522,17 +1543,16 @@
       <c r="H26" s="40"/>
       <c r="I26" s="40"/>
       <c r="J26" s="40"/>
-      <c r="K26" s="40"/>
+      <c r="K26" s="22"/>
       <c r="L26" s="22"/>
       <c r="M26" s="22"/>
       <c r="N26" s="22"/>
       <c r="O26" s="22"/>
       <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-    </row>
-    <row r="27" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="40"/>
       <c r="C27" s="40"/>
@@ -1549,11 +1569,10 @@
       <c r="N27" s="40"/>
       <c r="O27" s="40"/>
       <c r="P27" s="40"/>
-      <c r="Q27" s="40"/>
-    </row>
-    <row r="28" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28" s="40"/>
       <c r="C28" s="40"/>
@@ -1562,44 +1581,42 @@
       <c r="F28" s="40"/>
       <c r="G28" s="40"/>
       <c r="H28" s="40"/>
-      <c r="I28" s="40"/>
+      <c r="I28" s="22"/>
       <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="M28" s="8"/>
+      <c r="K28" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L28" s="8"/>
+      <c r="M28" s="22"/>
       <c r="N28" s="22"/>
       <c r="O28" s="22"/>
       <c r="P28" s="22"/>
-      <c r="Q28" s="22"/>
-    </row>
-    <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="22"/>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="8" t="s">
-        <v>22</v>
-      </c>
+      <c r="G29" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="23"/>
       <c r="I29" s="23"/>
       <c r="J29" s="23"/>
       <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="23"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="22"/>
       <c r="O29" s="22"/>
       <c r="P29" s="22"/>
-      <c r="Q29" s="22"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G30" s="20"/>
       <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="39"/>
       <c r="B31" s="39"/>
       <c r="C31" s="39"/>
@@ -1610,29 +1627,27 @@
       <c r="H31" s="39"/>
       <c r="I31" s="39"/>
       <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A5:N5"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A31:K31"/>
-    <mergeCell ref="A27:Q27"/>
-    <mergeCell ref="A28:I28"/>
-    <mergeCell ref="A26:K26"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="I14:M14"/>
-    <mergeCell ref="H14:H15"/>
+  <mergeCells count="18">
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="A27:P27"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="G14:G15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="F14:F15"/>
     <mergeCell ref="D14:D15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A6" r:id="rId1" location="/download"/>
@@ -1641,7 +1656,7 @@
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="84" orientation="landscape" r:id="rId2"/>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="15" max="1048575" man="1"/>
+    <brk id="14" max="1048575" man="1"/>
   </colBreaks>
   <drawing r:id="rId3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add a link to downlçoad
</commit_message>
<xml_diff>
--- a/documents/Model Feuille de pointages 2018.xlsx
+++ b/documents/Model Feuille de pointages 2018.xlsx
@@ -24,14 +24,14 @@
     <sheet name="Feuil10" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$N$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$A$1:$N$35</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>observation</t>
   </si>
@@ -45,13 +45,7 @@
     <t>N°</t>
   </si>
   <si>
-    <t>Sous toute résponssabilité de l'emploueur et de l'employé,</t>
-  </si>
-  <si>
     <t>Mois: ……………….../Année: ……………..</t>
-  </si>
-  <si>
-    <t>N° COMPTE</t>
   </si>
   <si>
     <t>Adresse:…………………………………………………………</t>
@@ -117,30 +111,6 @@
   </si>
   <si>
     <t>…………………….</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:les copies de justification (maladie,maternité,accident de travail...)doivent étre jointes au présent état et déposées au niveau de l'agence locale de l'emploi</t>
-    </r>
   </si>
   <si>
     <r>
@@ -223,12 +193,42 @@
   <si>
     <t>(**)Portez la mention appropriée:période de congé de maladie,maternité,accident de travail,congé annuel...ect</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:les copies de justification (maladie,maternité,accident de travail...) doivent étre jointes au présent état et déposées au niveau de l'agence locale de l'emploi</t>
+    </r>
+  </si>
+  <si>
+    <t>Sous toute résponssabilité de l'emploueur et de l'employé.</t>
+  </si>
+  <si>
+    <t>N° CCP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +326,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -509,7 +517,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -563,9 +571,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,7 +588,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -601,17 +612,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -643,8 +662,8 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>466724</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -668,7 +687,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10915650" cy="1219200"/>
+          <a:ext cx="10915650" cy="1419224"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -967,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P31"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -992,19 +1011,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="44"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
+      <c r="A1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
     </row>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
@@ -1051,33 +1070,31 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
+    <row r="5" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
     </row>
     <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -1096,11 +1113,11 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
+      <c r="A8" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="6"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -1113,14 +1130,14 @@
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
+      <c r="A9" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
       <c r="D9" s="6"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="34" t="s">
         <v>2</v>
       </c>
       <c r="I9" s="1"/>
@@ -1131,7 +1148,7 @@
     </row>
     <row r="10" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1148,7 +1165,7 @@
     </row>
     <row r="11" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1161,7 +1178,7 @@
     </row>
     <row r="12" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -1169,24 +1186,24 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="36" t="s">
-        <v>13</v>
+      <c r="H12" s="35" t="s">
+        <v>11</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="K12" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="L12" s="33" t="s">
-        <v>30</v>
+      <c r="J12" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="32" t="s">
+        <v>27</v>
       </c>
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1194,80 +1211,78 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="34"/>
+      <c r="H13" s="33"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:13" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="40" t="s">
+      <c r="B14" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="G14" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="H14" s="40" t="s">
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="41"/>
+      <c r="M14" s="40" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="40"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="39" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="L15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="M15" s="39"/>
+        <v>13</v>
+      </c>
+      <c r="M15" s="40"/>
     </row>
     <row r="16" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>1</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>27</v>
+      <c r="B16" s="47" t="s">
+        <v>25</v>
       </c>
       <c r="C16" s="11"/>
-      <c r="D16" s="12">
-        <v>43101</v>
-      </c>
+      <c r="D16" s="12"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
@@ -1282,8 +1297,8 @@
       <c r="A17" s="25">
         <v>2</v>
       </c>
-      <c r="B17" s="29" t="s">
-        <v>27</v>
+      <c r="B17" s="48" t="s">
+        <v>25</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="15"/>
@@ -1298,13 +1313,13 @@
       <c r="M17" s="15"/>
     </row>
     <row r="18" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30">
+      <c r="A18" s="29">
         <v>3</v>
       </c>
-      <c r="B18" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="31"/>
+      <c r="B18" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="30"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
@@ -1320,8 +1335,8 @@
       <c r="A19" s="25">
         <v>4</v>
       </c>
-      <c r="B19" s="29" t="s">
-        <v>27</v>
+      <c r="B19" s="48" t="s">
+        <v>25</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="15"/>
@@ -1339,8 +1354,8 @@
       <c r="A20" s="26">
         <v>5</v>
       </c>
-      <c r="B20" s="29" t="s">
-        <v>27</v>
+      <c r="B20" s="48" t="s">
+        <v>25</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="18"/>
@@ -1358,8 +1373,8 @@
       <c r="A21" s="16">
         <v>6</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>27</v>
+      <c r="B21" s="49" t="s">
+        <v>25</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -1377,8 +1392,8 @@
       <c r="A22" s="19">
         <v>7</v>
       </c>
-      <c r="B22" s="19" t="s">
-        <v>27</v>
+      <c r="B22" s="50" t="s">
+        <v>25</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
@@ -1396,8 +1411,8 @@
       <c r="A23" s="19">
         <v>8</v>
       </c>
-      <c r="B23" s="19" t="s">
-        <v>27</v>
+      <c r="B23" s="50" t="s">
+        <v>25</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -1411,58 +1426,57 @@
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
     </row>
-    <row r="24" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13">
+    <row r="24" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="16">
         <v>9</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
+      <c r="B24" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+    </row>
+    <row r="25" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="13">
+        <v>10</v>
+      </c>
+      <c r="B25" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
+      <c r="A26" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
       <c r="K26" s="22"/>
       <c r="L26" s="22"/>
       <c r="M26" s="22"/>
@@ -1471,94 +1485,113 @@
       <c r="P26" s="22"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="38"/>
-      <c r="N27" s="38"/>
-      <c r="O27" s="38"/>
-      <c r="P27" s="38"/>
+      <c r="A27" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="22"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="22"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
     </row>
     <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="L28" s="8"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
+      <c r="A28" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
+      <c r="O28" s="39"/>
+      <c r="P28" s="39"/>
     </row>
     <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="23"/>
+      <c r="A29" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="22"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L29" s="8"/>
+      <c r="M29" s="22"/>
       <c r="N29" s="22"/>
       <c r="O29" s="22"/>
       <c r="P29" s="22"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
+    <row r="30" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
-      <c r="B31" s="37"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+    </row>
+    <row r="32" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+      <c r="A32" s="44" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="44"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="44"/>
+      <c r="M32" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A5:M5"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="A27:P27"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A26:J26"/>
+  <mergeCells count="17">
+    <mergeCell ref="A28:P28"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A27:J27"/>
     <mergeCell ref="M14:M15"/>
     <mergeCell ref="H14:L14"/>
     <mergeCell ref="G14:G15"/>
@@ -1568,9 +1601,14 @@
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A32:M32"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A5:M5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" location="/download"/>
+    <hyperlink ref="A32" r:id="rId1" location="/download"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
Add 02 copies originales
</commit_message>
<xml_diff>
--- a/documents/Model Feuille de pointages 2018.xlsx
+++ b/documents/Model Feuille de pointages 2018.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>observation</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>Tél/Fax:……………………………………………………………….Email/………………………………………</t>
-  </si>
-  <si>
-    <t>Numéro d'immatriculation "CNAS"de l'organisme d'accueil:……………………………………………………………….</t>
   </si>
   <si>
     <t>Nbre de jours d'absence</t>
@@ -194,6 +191,15 @@
     <t>(**)Portez la mention appropriée:période de congé de maladie,maternité,accident de travail,congé annuel...ect</t>
   </si>
   <si>
+    <t>Sous toute résponssabilité de l'emploueur et de l'employé.</t>
+  </si>
+  <si>
+    <t>N° CCP</t>
+  </si>
+  <si>
+    <t>نسختين أصليتين (02)</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -214,14 +220,21 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>:les copies de justification (maladie,maternité,accident de travail...) doivent étre jointes au présent état et déposées au niveau de l'agence locale de l'emploi</t>
+      <t>:</t>
     </r>
-  </si>
-  <si>
-    <t>Sous toute résponssabilité de l'emploueur et de l'employé.</t>
-  </si>
-  <si>
-    <t>N° CCP</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>les copies de justification (maladie,maternité,accident de travail...) doivent étre jointes au présent état et déposées au niveau de l'agence locale de l'emploi</t>
+    </r>
+  </si>
+  <si>
+    <t>02 copies originales</t>
   </si>
 </sst>
 </file>
@@ -335,15 +348,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -512,12 +531,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -589,20 +638,17 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -619,18 +665,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -660,7 +711,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>781050</xdr:colOff>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>466724</xdr:rowOff>
     </xdr:to>
@@ -987,14 +1038,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
@@ -1010,19 +1061,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
+      <c r="A1" s="38"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
     </row>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
@@ -1070,19 +1121,19 @@
       <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="49"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
     </row>
     <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="35"/>
@@ -1101,11 +1152,11 @@
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
+      <c r="A7" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="6"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -1118,11 +1169,11 @@
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A8" s="50" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
+      <c r="A8" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
       <c r="D8" s="6"/>
       <c r="E8" s="8"/>
       <c r="F8" s="33" t="s">
@@ -1136,7 +1187,7 @@
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1175,24 +1226,22 @@
       <c r="F11" s="8"/>
       <c r="G11" s="1"/>
       <c r="H11" s="34" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="L11" s="31" t="s">
-        <v>27</v>
-      </c>
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
@@ -1205,69 +1254,69 @@
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:13" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="44" t="s">
+      <c r="G13" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="42"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="43" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="43"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M14" s="43"/>
+      <c r="M14" s="42"/>
     </row>
     <row r="15" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>1</v>
       </c>
-      <c r="B15" s="37" t="s">
-        <v>25</v>
+      <c r="B15" s="46" t="s">
+        <v>24</v>
       </c>
       <c r="C15" s="11"/>
       <c r="D15" s="12"/>
@@ -1285,8 +1334,8 @@
       <c r="A16" s="24">
         <v>2</v>
       </c>
-      <c r="B16" s="38" t="s">
-        <v>25</v>
+      <c r="B16" s="47" t="s">
+        <v>24</v>
       </c>
       <c r="C16" s="26"/>
       <c r="D16" s="15"/>
@@ -1304,8 +1353,8 @@
       <c r="A17" s="28">
         <v>3</v>
       </c>
-      <c r="B17" s="38" t="s">
-        <v>25</v>
+      <c r="B17" s="47" t="s">
+        <v>24</v>
       </c>
       <c r="C17" s="29"/>
       <c r="D17" s="17"/>
@@ -1323,8 +1372,8 @@
       <c r="A18" s="24">
         <v>4</v>
       </c>
-      <c r="B18" s="38" t="s">
-        <v>25</v>
+      <c r="B18" s="47" t="s">
+        <v>24</v>
       </c>
       <c r="C18" s="26"/>
       <c r="D18" s="15"/>
@@ -1342,8 +1391,8 @@
       <c r="A19" s="25">
         <v>5</v>
       </c>
-      <c r="B19" s="38" t="s">
-        <v>25</v>
+      <c r="B19" s="47" t="s">
+        <v>24</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="18"/>
@@ -1361,8 +1410,8 @@
       <c r="A20" s="16">
         <v>6</v>
       </c>
-      <c r="B20" s="39" t="s">
-        <v>25</v>
+      <c r="B20" s="48" t="s">
+        <v>24</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -1380,8 +1429,8 @@
       <c r="A21" s="19">
         <v>7</v>
       </c>
-      <c r="B21" s="40" t="s">
-        <v>25</v>
+      <c r="B21" s="49" t="s">
+        <v>24</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
@@ -1399,8 +1448,8 @@
       <c r="A22" s="19">
         <v>8</v>
       </c>
-      <c r="B22" s="40" t="s">
-        <v>25</v>
+      <c r="B22" s="49" t="s">
+        <v>24</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
@@ -1418,8 +1467,8 @@
       <c r="A23" s="19">
         <v>9</v>
       </c>
-      <c r="B23" s="40" t="s">
-        <v>25</v>
+      <c r="B23" s="49" t="s">
+        <v>24</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -1437,8 +1486,8 @@
       <c r="A24" s="13">
         <v>10</v>
       </c>
-      <c r="B24" s="41" t="s">
-        <v>25</v>
+      <c r="B24" s="50" t="s">
+        <v>24</v>
       </c>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
@@ -1454,7 +1503,7 @@
     </row>
     <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25" s="20"/>
       <c r="C25" s="20"/>
@@ -1473,18 +1522,18 @@
       <c r="P25" s="21"/>
     </row>
     <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
+      <c r="A26" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="41"/>
       <c r="K26" s="21"/>
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
@@ -1493,40 +1542,40 @@
       <c r="P26" s="21"/>
     </row>
     <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="42"/>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42"/>
-      <c r="N27" s="42"/>
-      <c r="O27" s="42"/>
-      <c r="P27" s="42"/>
-    </row>
-    <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
+      <c r="A27" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="41"/>
+      <c r="M27" s="41"/>
+      <c r="N27" s="41"/>
+      <c r="O27" s="41"/>
+      <c r="P27" s="41"/>
+    </row>
+    <row r="28" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
       <c r="I28" s="21"/>
       <c r="J28" s="21"/>
       <c r="K28" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L28" s="8"/>
       <c r="M28" s="21"/>
@@ -1534,15 +1583,19 @@
       <c r="O28" s="21"/>
       <c r="P28" s="21"/>
     </row>
-    <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
+      <c r="B29" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="52" t="s">
+        <v>32</v>
+      </c>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
       <c r="G29" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H29" s="22"/>
       <c r="I29" s="22"/>
@@ -1555,24 +1608,25 @@
       <c r="P29" s="21"/>
     </row>
     <row r="30" spans="1:16" ht="21" x14ac:dyDescent="0.35">
-      <c r="A30" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
-      <c r="K30" s="47"/>
-      <c r="L30" s="47"/>
-      <c r="M30" s="47"/>
+      <c r="A30" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="37"/>
+      <c r="K30" s="37"/>
+      <c r="L30" s="37"/>
+      <c r="M30" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A30:M30"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A5:M5"/>
@@ -1589,7 +1643,6 @@
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="D13:D14"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A30" r:id="rId1" location="/download"/>

</xml_diff>